<commit_message>
evaluate sensitivity of ODE correctness and performance to ODE solver tolerances; make tolerances an option for verify_model(); fix a couple of models; fix TestVerificationSuite
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/testing/semantic/00001/00001-wc_lang.xlsx
+++ b/tests/fixtures/verification/testing/semantic/00001/00001-wc_lang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6460" windowWidth="25200" windowHeight="9480" activeTab="8"/>
+    <workbookView xWindow="-54880" yWindow="24900" windowWidth="23460" windowHeight="8720" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4228,7 +4228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="192">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-12-05 17:09:36'</t>
   </si>
@@ -4798,6 +4798,12 @@
   </si>
   <si>
     <t>second^-1 * molecule^-1</t>
+  </si>
+  <si>
+    <t>density_c</t>
+  </si>
+  <si>
+    <t>gram / liter</t>
   </si>
 </sst>
 </file>
@@ -4914,7 +4920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4966,6 +4972,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7261,9 +7277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -7329,10 +7345,10 @@
         <v>182</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="D3" s="8">
+      <c r="D3" s="20">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="21">
         <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -7345,12 +7361,20 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="D4" s="22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E4" s="22">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -10365,9 +10389,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -10535,7 +10559,9 @@
       <c r="K4" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -11381,7 +11407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>

</xml_diff>

<commit_message>
retry verification of SSA simulations on failure -- assuming failure is rare, multiple failures likely indicate a real error; change default ODE tolerances to good tolerances for SBML test cases -- will need to be revised later; ensure that ODE solver prints all error messages; when plotting expected and actual simulation trajectories so that curves which are equal will both be visible; fix test_case_verifier; remove unused TIME_STEP_FACTOR
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/testing/semantic/00001/00001-wc_lang.xlsx
+++ b/tests/fixtures/verification/testing/semantic/00001/00001-wc_lang.xlsx
@@ -5,11 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/verification/testing/semantic/00001/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/verification/cases/semantic/00001/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-54880" yWindow="24900" windowWidth="23460" windowHeight="8720" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="1260" yWindow="10260" windowWidth="32320" windowHeight="5020" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1180" yWindow="15340" windowWidth="35880" windowHeight="6200" tabRatio="500" firstSheet="3" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4228,12 +4229,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="192">
-  <si>
-    <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-12-05 17:09:36'</t>
-  </si>
-  <si>
-    <t>!!ObjTables Type='TableOfContents' Description='Table of contents' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="209">
+  <si>
+    <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-12-05 16:22:38'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='TableOfContents' Description='Table of contents' Date='2019-12-05 16:22:38' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -4323,7 +4324,7 @@
     <t>!Revision</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Model' Name='Models' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Model' Name='Models' Date='2019-12-05 16:22:38' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Id</t>
@@ -4359,13 +4360,13 @@
     <t>!Created</t>
   </si>
   <si>
-    <t>2019-12-05 17:09:29</t>
+    <t>2019-12-05 16:22:32</t>
   </si>
   <si>
     <t>!Updated</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Taxon' Name='Taxons' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Taxon' Name='Taxons' Date='2019-12-05 16:22:38' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Rank</t>
@@ -4374,7 +4375,7 @@
     <t>!References</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Environment' Name='Environments' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Environment' Name='Environments' Date='2019-12-05 16:22:38' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Temperature</t>
@@ -4383,7 +4384,7 @@
     <t>!Temperature units</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Submodel' Name='Submodels' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Submodel' Name='Submodels' Date='2019-12-05 16:22:38' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Framework</t>
@@ -4395,7 +4396,7 @@
     <t>!Conclusions</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Compartment' Name='Compartments' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Compartment' Name='Compartments' Date='2019-12-05 16:22:38' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Initial volume</t>
@@ -4434,7 +4435,7 @@
     <t>!Initial density</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='SpeciesType' Name='Species types' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='SpeciesType' Name='Species types' Date='2019-12-05 16:22:38' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Structure</t>
@@ -4461,7 +4462,7 @@
     <t>!Type</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Species' Name='Species' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Species' Name='Species' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Species type</t>
@@ -4470,22 +4471,22 @@
     <t>!Compartment</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='DistributionInitConcentration' Name='Init species concentrations' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='DistributionInitConcentration' Name='Init species concentrations' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Species</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Observable' Name='Observables' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Observable' Name='Observables' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Expression</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Function' Name='Functions' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables Type='Data' Id='Reaction' Name='Reactions' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Function' Name='Functions' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Data' Id='Reaction' Name='Reactions' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Flux bounds</t>
@@ -4509,7 +4510,7 @@
     <t>!Maximum</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='RateLaw' Name='Rate laws' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='RateLaw' Name='Rate laws' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Reaction</t>
@@ -4518,7 +4519,7 @@
     <t>!Direction</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='DfbaObjective' Name='dFBA objectives' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='DfbaObjective' Name='dFBA objectives' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Reaction rate units</t>
@@ -4527,28 +4528,28 @@
     <t>!Coefficient units</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='DfbaObjReaction' Name='dFBA objective reactions' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='DfbaObjReaction' Name='dFBA objective reactions' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Cell size units</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='DfbaObjSpecies' Name='dFBA objective species' Date='2019-12-05 17:09:36' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='DfbaObjSpecies' Name='dFBA objective species' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!dFBA objective reaction</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Parameter' Name='Parameters' Date='2019-12-05 17:09:37' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Parameter' Name='Parameters' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Standard error</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='StopCondition' Name='Stop conditions' Date='2019-12-05 17:09:37' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables Type='Data' Id='Observation' Name='Observations' Date='2019-12-05 17:09:37' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='StopCondition' Name='Stop conditions' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Data' Id='Observation' Name='Observations' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Genotype</t>
@@ -4584,13 +4585,13 @@
     <t>!Experiment design</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='ObservationSet' Name='Observation sets' Date='2019-12-05 17:09:37' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='ObservationSet' Name='Observation sets' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Observations</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Conclusion' Name='Conclusions' Date='2019-12-05 17:09:37' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Conclusion' Name='Conclusions' Date='2019-12-05 16:22:39' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Process</t>
@@ -4602,7 +4603,7 @@
     <t>!Date</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Reference' Name='References' Date='2019-12-05 17:09:37' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Reference' Name='References' Date='2019-12-05 16:22:40' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Title</t>
@@ -4644,7 +4645,7 @@
     <t>!Pages</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Author' Name='Authors' Date='2019-12-05 17:09:37' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Author' Name='Authors' Date='2019-12-05 16:22:40' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Last name</t>
@@ -4668,7 +4669,7 @@
     <t>!Address</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Change' Name='Changes' Date='2019-12-05 17:09:37' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Change' Name='Changes' Date='2019-12-05 16:22:40' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Target</t>
@@ -4692,12 +4693,6 @@
     <t>!Intention type</t>
   </si>
   <si>
-    <t>test_case_00001</t>
-  </si>
-  <si>
-    <t>Basic single forward reaction</t>
-  </si>
-  <si>
     <t>ode_submodel</t>
   </si>
   <si>
@@ -4716,104 +4711,162 @@
     <t>cellular_compartment</t>
   </si>
   <si>
-    <t>fluid_compartment</t>
+    <t>gram</t>
   </si>
   <si>
     <t>normal_distribution</t>
   </si>
   <si>
-    <t>gram</t>
+    <t>l</t>
+  </si>
+  <si>
+    <t>density_c</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Equal MWs mass-balance the reactions</t>
+  </si>
+  <si>
+    <t>pseudo_species</t>
+  </si>
+  <si>
+    <t>S1[c]</t>
+  </si>
+  <si>
+    <t>S2[c]</t>
+  </si>
+  <si>
+    <t>molar</t>
+  </si>
+  <si>
+    <t>reaction_1</t>
+  </si>
+  <si>
+    <t>reaction 1</t>
+  </si>
+  <si>
+    <t>[c]: S1 ==&gt; S2</t>
+  </si>
+  <si>
+    <t>1 / second</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>k1</t>
+  </si>
+  <si>
+    <t>reaction_1-forward</t>
+  </si>
+  <si>
+    <t>taxon</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>domain not used</t>
+  </si>
+  <si>
+    <t>dist-init-conc-S1[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-S2[c]</t>
+  </si>
+  <si>
+    <t>s^-1</t>
+  </si>
+  <si>
+    <t>molecule</t>
+  </si>
+  <si>
+    <t>gram / liter</t>
+  </si>
+  <si>
+    <t>Basic single forward reaction with two species in one compartment</t>
+  </si>
+  <si>
+    <t>Density compartment c</t>
+  </si>
+  <si>
+    <t>Avogadro</t>
+  </si>
+  <si>
+    <t>molecule / mole</t>
+  </si>
+  <si>
+    <t>vol_c</t>
+  </si>
+  <si>
+    <t>Volume of compartment c</t>
   </si>
   <si>
     <t>liter</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>pseudo_species</t>
-  </si>
-  <si>
-    <t>Equal MWs mass-balance the reactions</t>
-  </si>
-  <si>
-    <t>S1[c]</t>
-  </si>
-  <si>
-    <t>S2[c]</t>
-  </si>
-  <si>
-    <t>molecule</t>
-  </si>
-  <si>
-    <t>molar</t>
-  </si>
-  <si>
-    <t>obs_1</t>
-  </si>
-  <si>
-    <t>2 * S1[c]</t>
-  </si>
-  <si>
-    <t>reaction_1</t>
-  </si>
-  <si>
-    <t>reaction 1</t>
-  </si>
-  <si>
-    <t>[c]: S1 ==&gt; S2</t>
-  </si>
-  <si>
-    <t>1 / second</t>
-  </si>
-  <si>
-    <t>forward</t>
-  </si>
-  <si>
-    <t>k1 * S1[c]</t>
-  </si>
-  <si>
-    <t>k1</t>
-  </si>
-  <si>
-    <t>reaction_1-forward</t>
-  </si>
-  <si>
-    <t>taxon</t>
-  </si>
-  <si>
-    <t>Test model</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>dist-init-conc-S1[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-S2[c]</t>
-  </si>
-  <si>
-    <t>second^-1 * molecule^-1</t>
-  </si>
-  <si>
-    <t>density_c</t>
-  </si>
-  <si>
-    <t>gram / liter</t>
+    <t>pop_2_conc</t>
+  </si>
+  <si>
+    <t>Convert population to concentration</t>
+  </si>
+  <si>
+    <t>1 / (Avogadro * vol_c)</t>
+  </si>
+  <si>
+    <t>mole / (molecule liter)</t>
+  </si>
+  <si>
+    <t>1 / mole</t>
+  </si>
+  <si>
+    <t>abstract_compartment</t>
+  </si>
+  <si>
+    <t>Same as specified in moles, as vol_c = 1 liter</t>
+  </si>
+  <si>
+    <t>k1 * S1[c] * pop_2_conc * vol_c * conv</t>
+  </si>
+  <si>
+    <t>conv</t>
+  </si>
+  <si>
+    <t>Conversion for rate law</t>
+  </si>
+  <si>
+    <t>Must equal volume of c in Compartments</t>
+  </si>
+  <si>
+    <t>Unit conversion for conv</t>
+  </si>
+  <si>
+    <t>1 / molecule</t>
+  </si>
+  <si>
+    <t>one_per_molecule</t>
+  </si>
+  <si>
+    <t>Avogadro * one_per_molecule</t>
+  </si>
+  <si>
+    <t>test_case_00001_pop_mass_independent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4852,6 +4905,21 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -4884,7 +4952,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -4916,11 +4984,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDA9694"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDA9694"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDA9694"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDA9694"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4944,15 +5031,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4960,12 +5047,85 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4973,18 +5133,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5286,10 +5440,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5574,10 +5729,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5628,15 +5785,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>172</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -5771,16 +5923,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5827,10 +5985,18 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>196</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -5838,12 +6004,20 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="33"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -5914,47 +6088,29 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:I2"/>
   <dataValidations count="9">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A3:A12">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A7:A10">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B7:B10">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="C3:C12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="D3:D12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="E3:E12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="F3:F12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="G3:G12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="H3:H12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="C7:C10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="D7:D10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="E7:E10"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="F7:F10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="G7:G10"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="H7:H10">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="I3:I12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="I7:I10"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5965,10 +6121,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6001,13 +6159,13 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="42" t="s">
         <v>86</v>
       </c>
       <c r="J2" s="5"/>
@@ -6062,22 +6220,22 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6237,7 +6395,7 @@
   <mergeCells count="1">
     <mergeCell ref="G2:I2"/>
   </mergeCells>
-  <dataValidations count="13">
+  <dataValidations count="14">
     <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A4:A13">
       <formula1>1</formula1>
       <formula2>63</formula2>
@@ -6249,7 +6407,7 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value_x000a__x000a_Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value_x000a__x000a_Select &quot;True&quot; or &quot;False&quot;." sqref="E4:E13">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="F4:F13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="F5:F13">
       <formula1>"1 / second"</formula1>
     </dataValidation>
     <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G4:G13">
@@ -6269,6 +6427,9 @@
       <formula1>4294967295</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N4:N13"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="F4">
+      <formula1>"1 / second"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6291,14 +6452,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="8" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6357,21 +6527,22 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -6463,83 +6634,38 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:L2"/>
-  <dataValidations count="13">
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A3:A12">
+  <dataValidations count="11">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B5:B9">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D4:D12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A5:A9">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D5:D9">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E3:E12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E5:E9">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F4:F12"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="G4:G12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F5:F9"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="G5:G9">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H3:H12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I3:I12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J3:J12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K3:K12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H5:H9"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I5:I9"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J5:J9"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K5:K9">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L3:L12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B4:B12 D3">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="C3">
-      <formula1>1</formula1>
-      <formula2>63</formula2>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="G3">
-      <formula1>"1 / second"</formula1>
-    </dataValidation>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L5:L9"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -6548,7 +6674,7 @@
           <x14:formula1>
             <xm:f>'!!Reactions'!$A$4:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C12 F3</xm:sqref>
+          <xm:sqref>C5:C9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6560,10 +6686,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6813,10 +6940,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7035,10 +7163,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7277,16 +7406,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:E4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="38" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="32" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7296,8 +7434,8 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -7306,22 +7444,22 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="21" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -7341,18 +7479,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="D3" s="20">
+      <c r="A3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="35">
         <v>1</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="26">
         <v>0</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>189</v>
+      <c r="F3" s="28" t="s">
+        <v>174</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -7362,18 +7501,20 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>163</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>187</v>
+      </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="22">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E4" s="22">
+      <c r="D4" s="36">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>191</v>
+      <c r="F4" s="24" t="s">
+        <v>185</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -7382,12 +7523,20 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="37">
+        <v>6.0221408570000002E+23</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>189</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -7395,25 +7544,47 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="40">
+        <v>1</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>192</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="22" t="s">
+        <v>203</v>
+      </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>204</v>
+      </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="36">
+        <v>1</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>205</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -7424,8 +7595,8 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -7437,8 +7608,8 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -7450,8 +7621,8 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -7459,58 +7630,34 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:K2"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A3:A12">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A9:A10">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B9:B10">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C3:C12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C9:C10">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D4:D12">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D9:D10">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="F3:F12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G3:G12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="H3:H12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I3:I12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="J3:J12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="F9:F10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G9:G10"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="H9:H10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I9:I10"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="J9:J10">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K3:K12"/>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E4:E12 D3">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K9:K10"/>
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E9:E10">
       <formula1>-1E-100</formula1>
     </dataValidation>
   </dataValidations>
@@ -7523,10 +7670,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7717,10 +7865,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7762,42 +7911,42 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="42" t="s">
         <v>108</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="19" t="s">
+      <c r="R2" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="S2" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="T2" s="42" t="s">
         <v>110</v>
       </c>
       <c r="U2" s="5"/>
@@ -8210,12 +8359,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8245,7 +8395,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>154</v>
+        <v>208</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8263,7 +8413,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -8447,25 +8597,7 @@
       <c r="L13" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="12">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="B2:L2">
-      <formula1>1</formula1>
-      <formula2>63</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:L3">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Version" error="Value must be a string." promptTitle="Version" prompt="Enter a string." sqref="B4:L4"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="URL" error="Enter a valid URL_x000a__x000a_Value must be a string._x000a__x000a_Value must be less than or equal to 65535 characters." promptTitle="URL" prompt="Enter a valid URL_x000a__x000a_Enter a string._x000a__x000a_Value must be less than or equal to 65535 characters." sqref="B5:L5">
-      <formula1>65535</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B6:L6">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B7:L7">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="wc_lang version" error="Value must be a string." promptTitle="wc_lang version" prompt="Enter a string." sqref="B8:L8"/>
+  <dataValidations count="5">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Time units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;second&quot; or blank." promptTitle="Time units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;second&quot; or blank." sqref="B9:L9">
       <formula1>"second"</formula1>
     </dataValidation>
@@ -8491,10 +8623,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8638,10 +8771,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8674,10 +8808,10 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="42" t="s">
         <v>121</v>
       </c>
       <c r="I2" s="5"/>
@@ -8941,10 +9075,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9296,10 +9431,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9556,6 +9692,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9897,13 +10034,15 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="11" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="8.83203125" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9926,8 +10065,8 @@
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>184</v>
+      <c r="B2" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9943,9 +10082,7 @@
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>185</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -9960,8 +10097,8 @@
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>186</v>
+      <c r="B4" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -9992,7 +10129,9 @@
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -10048,6 +10187,7 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10206,8 +10346,9 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10255,15 +10396,14 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -10272,7 +10412,6 @@
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -10369,16 +10508,16 @@
     <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Framework" error="Value must be a comma-separated list of WC ontology terms &quot;deterministic_simulation_algorithm&quot;, &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." promptTitle="Framework" prompt="Enter a comma-separated list of WC ontology terms &quot;deterministic_simulation_algorithm&quot;, &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." sqref="C3:C12">
-      <formula1>"deterministic_simulation_algorithm,dynamic_flux_balance_analysis,ordinary_differential_equations,stochastic_simulation_algorithm"</formula1>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="D3:D12"/>
     <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="E3:E12"/>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="F3:F12"/>
     <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="G3:G12">
       <formula1>4294967295</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="H3:H12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="D4:D12"/>
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Framework" error="Value must be a comma-separated list of WC ontology terms &quot;deterministic_simulation_algorithm&quot;, &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." promptTitle="Framework" prompt="Enter a comma-separated list of WC ontology terms &quot;deterministic_simulation_algorithm&quot;, &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." sqref="C5:C12 C3">
+      <formula1>"deterministic_simulation_algorithm,dynamic_flux_balance_analysis,ordinary_differential_equations,stochastic_simulation_algorithm"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -10389,10 +10528,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10433,29 +10573,29 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="42" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="P2" s="42" t="s">
         <v>57</v>
       </c>
       <c r="Q2" s="5"/>
@@ -10531,36 +10671,36 @@
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>160</v>
-      </c>
       <c r="C4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E4" s="10"/>
+        <v>159</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="I4" s="10">
+        <v>160</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" s="9">
         <v>1</v>
       </c>
       <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>190</v>
+      <c r="K4" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -10580,11 +10720,8 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="10"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -10756,7 +10893,29 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+    </row>
   </sheetData>
   <autoFilter ref="A3:U3"/>
   <mergeCells count="2">
@@ -10764,63 +10923,69 @@
     <mergeCell ref="M2:P2"/>
   </mergeCells>
   <dataValidations count="18">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A4:A12">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A4:A13">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B4:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B4:B13">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological type" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." sqref="C4:C12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological type" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." sqref="C4:C13">
       <formula1>"cellular_compartment,extracellular_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D4:D12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D5:D13">
       <formula1>"fluid_compartment,membrane_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Geometry" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." sqref="E4:E12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Geometry" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." sqref="E4:E13">
       <formula1>"3D_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Parent compartment" error="Value must be a value from &quot;!!Compartments:A&quot; or blank." promptTitle="Parent compartment" prompt="Select a value from &quot;!!Compartments:A&quot; or blank." sqref="F4:F12">
-      <formula1>$A$4:$A$1048576</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mass units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;gram&quot; or blank." promptTitle="Mass units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;gram&quot; or blank." sqref="G4:G12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mass units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;gram&quot; or blank." promptTitle="Mass units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;gram&quot; or blank." sqref="G4:G13">
       <formula1>"gram"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="M4:M12 H4:H12"/>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="I4:I12">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="I4:I13">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="O4:O12 J4:J12">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="J4:J13 O4:O13">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;liter&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;liter&quot; or blank." sqref="K4:K12">
-      <formula1>"liter"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank." sqref="N4:N12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="M4:M13 H4 H6:H13"/>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank." sqref="N4:N13">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;dimensionless&quot; or blank." sqref="P4:P12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;dimensionless&quot; or blank." sqref="P4:P13">
       <formula1>"dimensionless"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="Q4:Q12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="R4:R12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="S4:S12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="T4:T12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="Q4:Q13"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="R4:R13"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="S4:S13"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="T4:T13">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="U4:U12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="U4:U13"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;liter&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;liter&quot; or blank." sqref="K6:K13 K4">
+      <formula1>"liter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Parent compartment" error="Value must be a value from &quot;!!Compartments:A&quot; or blank." promptTitle="Parent compartment" prompt="Select a value from &quot;!!Compartments:A&quot; or blank." sqref="F4:F13">
+      <formula1>$A$4:$A$1048576</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Initial density" error="Value must be a value from &quot;!!Parameters:A&quot; or blank." promptTitle="Initial density" prompt="Select a value from &quot;!!Parameters:A&quot; or blank.">
           <x14:formula1>
             <xm:f>'!!Parameters'!$A$3:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>L4:L12</xm:sqref>
+          <xm:sqref>L6:L13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Initial density" error="Value must be a value from &quot;!!Parameters:A&quot; or blank." promptTitle="Initial density" prompt="Select a value from &quot;!!Parameters:A&quot; or blank.">
+          <x14:formula1>
+            <xm:f>'!!Parameters'!$A$3:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10832,14 +10997,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="14" width="15.6640625" customWidth="1"/>
+    <col min="1" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10864,22 +11033,22 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="42" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="5"/>
@@ -10889,7 +11058,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -10935,55 +11104,57 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="8">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="3">
         <v>0</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>168</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="8">
+      <c r="G5" s="3">
         <v>1</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="3">
         <v>0</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>168</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N5" s="3"/>
     </row>
@@ -11146,13 +11317,13 @@
       <formula2>32767</formula2>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;I ..." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;Ion&quot;, &quot;am ..." sqref="I4:I13"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J4:J13"/>
     <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="K4:K13"/>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L4:L13"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="M6:M13">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="M4:M13">
       <formula1>4294967295</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N4:N13"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J6:J13 M4:M5"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11163,10 +11334,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11222,17 +11395,17 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -11242,17 +11415,17 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -11358,7 +11531,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:J2"/>
-  <dataValidations count="9">
+  <dataValidations count="8">
     <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A3:A12">
       <formula1>255</formula1>
     </dataValidation>
@@ -11375,10 +11548,6 @@
       <formula1>4294967295</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="J3:J12"/>
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="C3:C4">
-      <formula1>1</formula1>
-      <formula2>63</formula2>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11389,7 +11558,7 @@
           <x14:formula1>
             <xm:f>'!!Species types'!$A$4:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C12</xm:sqref>
+          <xm:sqref>C3:C12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Compartment" error="Value must be a value from &quot;!!Compartments:A&quot;." promptTitle="Compartment" prompt="Select a value from &quot;!!Compartments:A&quot;.">
           <x14:formula1>
@@ -11407,14 +11576,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="15.6640625" customWidth="1"/>
+    <col min="1" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="32.5" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11434,7 +11607,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -11474,54 +11647,58 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>170</v>
-      </c>
-      <c r="D3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="15">
-        <v>1.4999999999999999E-4</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="K3" s="22" t="s">
+        <v>199</v>
+      </c>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E4" s="14">
         <v>0</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="15">
         <v>0</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>173</v>
+      <c r="G4" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="22" t="s">
+        <v>199</v>
+      </c>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11639,29 +11816,29 @@
   </sheetData>
   <autoFilter ref="A2:L2"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A3:A12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A6:A12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B6:B12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E5:E12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D6:D12"/>
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E6:E12">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="F3:F12">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="F6:F12">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G3:G12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G6:G12">
       <formula1>"molecule,molar,millimolar,micromolar,nanomolar,picomolar,femtomolar,attomolar"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H3:H12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I3:I12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J3:J12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K3:K12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H6:H12"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I6:I12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J6:J12"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K6:K12">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L3:L12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D5:D12 E3:E4"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L6:L12"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11672,7 +11849,7 @@
           <x14:formula1>
             <xm:f>'!!Species'!$A$3:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C12</xm:sqref>
+          <xm:sqref>C6:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>